<commit_message>
Würzburg Karte: Design modernisiert und Standard-Marker implementiert
</commit_message>
<xml_diff>
--- a/geodaten_template.xlsx
+++ b/geodaten_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Moritz\Documents\GitHub\Hangover-WUEedition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C2500F3-71A0-4A25-B408-E6E87B8CA4A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50C4D35-768A-4F42-8E5A-36CA7EF80207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -1594,9 +1594,9 @@
     <col min="7" max="7" width="31.9296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="38.53125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.9296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="1" customWidth="1"/>
     <col min="11" max="11" width="9.796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.45">
@@ -3375,5 +3375,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>